<commit_message>
just updated script filesfiles.
</commit_message>
<xml_diff>
--- a/TestScripts/Outputs/nsx-payload.xlsx
+++ b/TestScripts/Outputs/nsx-payload.xlsx
@@ -2,18 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <bookViews>
-    <workbookView/>
+    <workbookView activeTab="-1"/>
   </bookViews>
   <sheets>
-    <sheet name="NSXEdges" sheetId="15" r:id="rId16"/>
-    <sheet name="NSXVirtServers" sheetId="16" r:id="rId17"/>
+    <sheet name="NSXEdges" sheetId="1" r:id="rId3"/>
+    <sheet name="NSXVirtServers" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="348">
   <si>
     <t>id</t>
   </si>
@@ -228,36 +228,6 @@
     <t>vse-06ccf82e-b987-424a-be87-ba2d12e37509</t>
   </si>
   <si>
-    <t>edge-125</t>
-  </si>
-  <si>
-    <t>fd34313f-3a71-4831-b056-c280c2ee5afa</t>
-  </si>
-  <si>
-    <t>vse-Nasosenergoprom EDGE (18ae003c-0bf3-499b-8f40-9e763ec55c95)</t>
-  </si>
-  <si>
-    <t>vse-f363900a-44a7-45ce-a26b-adb428ace8d6</t>
-  </si>
-  <si>
-    <t>Nasosenergoprom</t>
-  </si>
-  <si>
-    <t>edge-127</t>
-  </si>
-  <si>
-    <t>5ff945bb-402d-4181-9b83-0e64e17e7ee9</t>
-  </si>
-  <si>
-    <t>vse-Teplyidim EDGE (a4c09dce-cfea-4684-80f0-ca600f6523ee)</t>
-  </si>
-  <si>
-    <t>vse-f4e6c17c-e031-42d0-9466-03bbc6f4af20</t>
-  </si>
-  <si>
-    <t>КП "Теплий Дім", Test from 22.12.2020, Taras Melnik, +3805033834328, iks.miuk@gmail.com</t>
-  </si>
-  <si>
     <t>edge-128</t>
   </si>
   <si>
@@ -303,21 +273,6 @@
     <t xml:space="preserve">Mirs		 Виталий Стратинский		 itd@tango.com.ua		</t>
   </si>
   <si>
-    <t>edge-134</t>
-  </si>
-  <si>
-    <t>e9dbe5e7-3062-496e-b984-d611745905f9</t>
-  </si>
-  <si>
-    <t>vse-Novofarm EDGE (dd338247-4b56-4050-8985-025546cdadad)</t>
-  </si>
-  <si>
-    <t>vse-f39aaba0-7037-4f3c-b17f-a8446db4de6e</t>
-  </si>
-  <si>
-    <t>Novofarm</t>
-  </si>
-  <si>
     <t>edge-136</t>
   </si>
   <si>
@@ -405,51 +360,6 @@
     <t>33m2 Edge</t>
   </si>
   <si>
-    <t>edge-145</t>
-  </si>
-  <si>
-    <t>28e694f6-12ff-44dc-a8bf-12e37a80fd42</t>
-  </si>
-  <si>
-    <t>vse-KTCM Edge (90abfb5d-1a7a-4292-af7f-b8acb93ec8fc)</t>
-  </si>
-  <si>
-    <t>vse-04ea64f1-decc-4d55-98f5-1b773e0069e4</t>
-  </si>
-  <si>
-    <t>KTCM Edge</t>
-  </si>
-  <si>
-    <t>edge-146</t>
-  </si>
-  <si>
-    <t>f60a8436-2334-4c68-b6c2-6cd44f00f00f</t>
-  </si>
-  <si>
-    <t>vse-MVPO Edge (3afa3225-cae2-45cd-afa9-5a8bd0109761)</t>
-  </si>
-  <si>
-    <t>vse-5660fc2b-035e-44bd-a8f3-52608ef5c10b</t>
-  </si>
-  <si>
-    <t>MVPO Edge</t>
-  </si>
-  <si>
-    <t>edge-147</t>
-  </si>
-  <si>
-    <t>18c3c4f8-b002-44a4-a943-9f59369eb6ab</t>
-  </si>
-  <si>
-    <t>vse-Netreba EDGE (f8f8da34-d713-4d38-81eb-a979d30bc657)</t>
-  </si>
-  <si>
-    <t>vse-ddff71d2-0ac8-473b-9de5-4f91c856b76f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ФОП "Нетреба О.В."		 netreba		 Колесник Дмитрий Викторович		 </t>
-  </si>
-  <si>
     <t>edge-148</t>
   </si>
   <si>
@@ -495,51 +405,6 @@
     <t>ООО "Ясенсвит"</t>
   </si>
   <si>
-    <t>edge-152</t>
-  </si>
-  <si>
-    <t>1583b5f4-ef7c-400c-a267-1883793b6875</t>
-  </si>
-  <si>
-    <t>vse-Bdcloud EDGE (b5662084-30e6-41fe-bebf-8f8b745317ab)</t>
-  </si>
-  <si>
-    <t>vse-3072e14c-f47e-4e36-886c-438ce1812070</t>
-  </si>
-  <si>
-    <t>Bdcloud EDGE</t>
-  </si>
-  <si>
-    <t>edge-153</t>
-  </si>
-  <si>
-    <t>caa867a1-2dac-475f-8ed3-28c6978d61ac</t>
-  </si>
-  <si>
-    <t>vse-NPP EDGE (8e5e795e-6dc3-411f-83aa-fcc7a44d99de)</t>
-  </si>
-  <si>
-    <t>vse-14e312a3-4ea9-41ed-9225-a61968ab67b4</t>
-  </si>
-  <si>
-    <t>"Запорожская АЭС" TEST 17.03.2021 Белоус Денис Васильевич, oit6556@mgw.npp.zp.ua, +380509164329</t>
-  </si>
-  <si>
-    <t>edge-154</t>
-  </si>
-  <si>
-    <t>9d223951-8ecf-4f60-a6f9-8530494b883a</t>
-  </si>
-  <si>
-    <t>vse-JUMP EDGE (7b70f430-dc68-4290-86f6-8abb492c569d)</t>
-  </si>
-  <si>
-    <t>vse-e846b70b-ad40-48ef-a8a5-872d7612a8ea</t>
-  </si>
-  <si>
-    <t>Jump</t>
-  </si>
-  <si>
     <t>edge-155</t>
   </si>
   <si>
@@ -567,52 +432,7 @@
     <t>vse-49d6373c-e5ae-4ac8-8eec-c79996860688</t>
   </si>
   <si>
-    <t>ТОВ "НАДЕЖДА РИТЕЙЛ 2017" Test start from 23.03.2021 Parfilev Valerii, +380503009496, pvi@oil.pl.ua</t>
-  </si>
-  <si>
-    <t>edge-157</t>
-  </si>
-  <si>
-    <t>efe1ed35-b5f2-48da-b646-140aa8df469a</t>
-  </si>
-  <si>
-    <t>vse-OrionUgMK EDGE (a281ff98-3034-4e3f-8074-95720d0543b2)</t>
-  </si>
-  <si>
-    <t>vse-53fa4954-a632-4173-8cf3-a359056fce10</t>
-  </si>
-  <si>
-    <t>OrionUgMK TEST 26.03.21</t>
-  </si>
-  <si>
-    <t>edge-159</t>
-  </si>
-  <si>
-    <t>47ca2188-bc39-47ef-ba8f-27561df3a07e</t>
-  </si>
-  <si>
-    <t>vse-Comex EDGE (4165e19b-483b-4ae6-bd80-6f495c83b359)</t>
-  </si>
-  <si>
-    <t>vse-1b882f6c-ed3a-4b25-8405-8be514995692</t>
-  </si>
-  <si>
-    <t>ООО "Металлоцентры Комэкс", TEST 29.03.2021 Олейник С.В., stas.masterok@gmail.com, +380506090909</t>
-  </si>
-  <si>
-    <t>edge-160</t>
-  </si>
-  <si>
-    <t>4f00a51b-7981-4191-89bf-022585f0ea71</t>
-  </si>
-  <si>
-    <t>vse-Vitiaz (e57bc174-f0a8-4a97-be6a-2470b582db10)</t>
-  </si>
-  <si>
-    <t>vse-ee08a89e-de84-41f1-a703-a5ecac79f050</t>
-  </si>
-  <si>
-    <t>Vitiaz, TEST 31.03.21</t>
+    <t xml:space="preserve">ТОВ "НАДЕЖДА РИТЕЙЛ 2017" PROD. Start  from 01.05.2021 (Test start from 23.03.2021) Parfilev Valerii, +380503009496, pvi@oil.pl.ua</t>
   </si>
   <si>
     <t>edge-161</t>
@@ -639,21 +459,6 @@
     <t>vse-43497c83-fa48-4322-ab6f-c225cd2bf7cc</t>
   </si>
   <si>
-    <t>edge-163</t>
-  </si>
-  <si>
-    <t>305fecd0-0ffb-44c4-962c-12e2447bcf6d</t>
-  </si>
-  <si>
-    <t>vse-Paycenter EDGE (87fe4416-9178-4a95-88fb-e7cd0519d299)</t>
-  </si>
-  <si>
-    <t>vse-1b526c5d-3938-41ec-8aaa-264c99658084</t>
-  </si>
-  <si>
-    <t>Paycenter</t>
-  </si>
-  <si>
     <t>edge-164</t>
   </si>
   <si>
@@ -669,15 +474,6 @@
     <t xml:space="preserve">"Регіональна газова компанія" PROD 14.04.2021 Александр Грекалов	050-425-33-37	Oleksandr.Grekalov@rgk.ua</t>
   </si>
   <si>
-    <t>edge-165</t>
-  </si>
-  <si>
-    <t>vse-vlan13 (c9f07a65-1196-4c20-b135-66c2e961b52e)</t>
-  </si>
-  <si>
-    <t>vse-c9f07a65-1196-4c20-b135-66c2e961b52e</t>
-  </si>
-  <si>
     <t>edge-166</t>
   </si>
   <si>
@@ -738,46 +534,484 @@
     <t xml:space="preserve">Wicken  TEST 23.04.21</t>
   </si>
   <si>
-    <t>edge-171</t>
-  </si>
-  <si>
-    <t>a2649d44-9036-4b81-8c3e-e2847e0581ae</t>
-  </si>
-  <si>
-    <t>vse-VAT_SHRBU65 EDGE (168a125e-08aa-444c-a809-4e404f876be2)</t>
-  </si>
-  <si>
-    <t>vse-756c5d5d-c068-4e33-b08e-aab1f00c671e</t>
-  </si>
-  <si>
-    <t>VAT_SHRBU65, TEST 28.04.21</t>
-  </si>
-  <si>
-    <t>edge-172</t>
-  </si>
-  <si>
-    <t>a8e80c92-e7e6-4198-aef3-15abb3a0ce8c</t>
-  </si>
-  <si>
-    <t>vse-Mlyn EDGE (d54f5fe2-d571-4988-b900-c3b281784f58)</t>
-  </si>
-  <si>
-    <t>vse-38b063dc-765f-4413-8620-64ca60b5ece6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ТОВ "Хмельницьк-млин" , TEST start from 28.04.2021,  Andrey Rovensky, +380503767288, rovic@mlyn.km.ua</t>
-  </si>
-  <si>
-    <t>edge-174</t>
-  </si>
-  <si>
-    <t>2b92dd0e-7421-492f-a10a-c9cb0250ad88</t>
-  </si>
-  <si>
-    <t>vse-Florian EDGE (9fb12197-48c1-4aa6-88b1-8a2fbbfb5cf8)</t>
-  </si>
-  <si>
-    <t>vse-730c6b02-6eff-45f1-8963-c3bbe5adbf67</t>
+    <t>edge-178</t>
+  </si>
+  <si>
+    <t>441423ac-8101-406d-b618-b7ef0801a530</t>
+  </si>
+  <si>
+    <t>vse-TB_UHT EDGE (16adb448-ac6f-4b99-be81-1a3390980f01)</t>
+  </si>
+  <si>
+    <t>vse-d9d4840d-5483-49c7-a638-338b6458e528</t>
+  </si>
+  <si>
+    <t>TB_UHT, TEST 14.05.21</t>
+  </si>
+  <si>
+    <t>edge-179</t>
+  </si>
+  <si>
+    <t>b3da94bd-e9ac-4e88-91a9-3f276becb3ca</t>
+  </si>
+  <si>
+    <t>vse-LogicTrail EDGE (4fd91e1e-3046-44ca-84dd-9b5acaed3508)</t>
+  </si>
+  <si>
+    <t>vse-64d216ba-25ee-48db-a7ab-8268123c9ccc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LogicTrail,  TEST 17.05.21</t>
+  </si>
+  <si>
+    <t>edge-181</t>
+  </si>
+  <si>
+    <t>d69479f2-46be-4ee3-94cb-9cd7acb73147</t>
+  </si>
+  <si>
+    <t>vse-MARTIN_LLC EDGE (6ac067b1-88bf-4f4b-a3b3-a384456d991a)</t>
+  </si>
+  <si>
+    <t>vse-2bcb4684-241c-437a-a7da-28f7e2794de9</t>
+  </si>
+  <si>
+    <t>MARTIN_LLC, TEST 17.05.21</t>
+  </si>
+  <si>
+    <t>edge-183</t>
+  </si>
+  <si>
+    <t>86494807-13fb-470d-b350-1be54ac35408</t>
+  </si>
+  <si>
+    <t>vse-CooperativLV EDGE (5a34033e-5e22-4473-853e-152df45a947e)</t>
+  </si>
+  <si>
+    <t>vse-d514d9f9-524f-43f1-9328-f05d6ed96916</t>
+  </si>
+  <si>
+    <t>"CooperativLV". TEST start 18.05.2021 Yakonyuk Ruslan, +380504476553, supermagik007@gmail.com</t>
+  </si>
+  <si>
+    <t>edge-185</t>
+  </si>
+  <si>
+    <t>ff26a6d2-6c09-4865-93f0-daba7acc3120</t>
+  </si>
+  <si>
+    <t>vse-Chertaras EDGE (9d2400f7-a471-4cf5-9e69-9ba4b01c2157)</t>
+  </si>
+  <si>
+    <t>vse-21e461db-6bc2-4427-a867-5dab080a99c0</t>
+  </si>
+  <si>
+    <t>ТОВ "Демидівський граніт" TEST 24.05.2021 Чернюк Тарас Вікторович chertaras2017@gmail.com, 068-0804892</t>
+  </si>
+  <si>
+    <t>edge-186</t>
+  </si>
+  <si>
+    <t>3f4e0abd-5f88-42b7-b83a-b45425eb420d</t>
+  </si>
+  <si>
+    <t>vse-Korostyshivgas EDGE (335df357-41c4-45f2-88a7-b462f6390cca)</t>
+  </si>
+  <si>
+    <t>vse-3ebe31c3-e7a2-4b81-b575-84c8596013f0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ПРАТ "КОРОСТИШІВГАЗ"  Test 24.05.2021 Рудаков Ігор Михайлович, ir040534@gmail.com, 0971863512</t>
+  </si>
+  <si>
+    <t>edge-187</t>
+  </si>
+  <si>
+    <t>b6f1ef47-761e-46f1-a805-011628099d03</t>
+  </si>
+  <si>
+    <t>vse-OMEGAHFK EDGE (d3618e82-111c-456b-9f24-b6ae6f57fff2)</t>
+  </si>
+  <si>
+    <t>vse-866c0d24-9a0c-46bc-ad78-3345af34aadd</t>
+  </si>
+  <si>
+    <t>ТОВ"ОМЕГА ХФК" Test 24.05.21 Кононенко Олег, oleg.konon@gmail.com, 0503085842</t>
+  </si>
+  <si>
+    <t>edge-188</t>
+  </si>
+  <si>
+    <t>60b896fa-cf26-4847-8a3c-bb6fe0cfc9d7</t>
+  </si>
+  <si>
+    <t>vse-Zhytomyrskykartony EDGE (994633f8-fdc7-4d96-a84e-d8f12267b3cc)</t>
+  </si>
+  <si>
+    <t>vse-cca59105-4389-42d3-b140-3097569cafb0</t>
+  </si>
+  <si>
+    <t>ТОВ "ЖИТОМИРСЬКИЙ КАРТОННИЙ КОМБІНАТ" Test 24.05.2021 Мисюра Олександр Вікторович, Oleksandr.Lysiura@cardboard.com.ua, 0665030553</t>
+  </si>
+  <si>
+    <t>edge-189</t>
+  </si>
+  <si>
+    <t>000b29ce-2986-40bc-87c3-161564053193</t>
+  </si>
+  <si>
+    <t>vse-Talamus EDGE (604e93f9-341f-438f-bd76-93813889bff1)</t>
+  </si>
+  <si>
+    <t>vse-f7e412e0-2775-4913-a249-daff769f9475</t>
+  </si>
+  <si>
+    <t>Talamus</t>
+  </si>
+  <si>
+    <t>edge-190</t>
+  </si>
+  <si>
+    <t>e5bb3bcf-9b66-4314-a0a9-b1284440e21c</t>
+  </si>
+  <si>
+    <t>vse-Petroline EDGE (24844f15-7fe9-41d3-b406-a6a6f756c2cb)</t>
+  </si>
+  <si>
+    <t>vse-79205b2f-1e56-4dbb-9e8d-f24d2ae3ca01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"Petroline", TEST start from 26.05.2021,  Yurii Juravlov, +380934807282, rsx1993@gmail.com</t>
+  </si>
+  <si>
+    <t>edge-191</t>
+  </si>
+  <si>
+    <t>4600e08f-5f7b-4898-a03f-0890c3f72ecf</t>
+  </si>
+  <si>
+    <t>vse-KOROSTENSKY_CAREER EDGE (5c7b8657-b9d0-45d6-8346-9fea21e4298a)</t>
+  </si>
+  <si>
+    <t>vse-0968aaf7-9cc1-4d74-9c07-fadde70567f9</t>
+  </si>
+  <si>
+    <t>KOROSTENSKY_CAREER, TEST04.06.21</t>
+  </si>
+  <si>
+    <t>edge-193</t>
+  </si>
+  <si>
+    <t>c7b6fb51-c01a-44c6-a5ba-f352137af6a7</t>
+  </si>
+  <si>
+    <t>vse-Oblik_online EDGE (5f90b87e-54d4-464a-89e2-5eeefd43b5e9)</t>
+  </si>
+  <si>
+    <t>vse-a7bc2896-1b7d-4e51-a391-ac1ba3da4b45</t>
+  </si>
+  <si>
+    <t>Oblik_online, TEST 04.06.21</t>
+  </si>
+  <si>
+    <t>edge-194</t>
+  </si>
+  <si>
+    <t>44a15b1d-fdda-475a-87ae-7cb9ea488fd5</t>
+  </si>
+  <si>
+    <t>vse-Dererom EDGE (a0db2303-05ec-4dc7-a9a3-35467e2cf47d)</t>
+  </si>
+  <si>
+    <t>vse-24c34298-5ab8-4ded-b889-9a9bdc591fe3</t>
+  </si>
+  <si>
+    <t>"Иноватив транспорт компани", TEST start from 07.06.2021, Roman K., +380503342233, dererom@gmail.com</t>
+  </si>
+  <si>
+    <t>edge-196</t>
+  </si>
+  <si>
+    <t>f118f059-5012-476d-b3fc-acb00dda6c4b</t>
+  </si>
+  <si>
+    <t>vse-Document Edge (bc1a4f58-4c74-4d38-a8bf-974a69fcdb5f)</t>
+  </si>
+  <si>
+    <t>vse-6ffb3aff-3f91-45c6-873a-6987578ca83c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ДП “Документ” Test 10.06.21 Хаврюченко Роман Петрович   romich1309@gmail.com; r_khavryuchenko@dpdok.com.ua  +380639755978</t>
+  </si>
+  <si>
+    <t>edge-197</t>
+  </si>
+  <si>
+    <t>e1c32a71-e1fb-4575-85c0-7588e427e45a</t>
+  </si>
+  <si>
+    <t>vse-Galpidshypnyk_com EDGE (1654cc4e-8ba5-426e-ad10-5bda91e9f167)</t>
+  </si>
+  <si>
+    <t>vse-a7a7f6bd-d751-44f0-8323-96557a86fe21</t>
+  </si>
+  <si>
+    <t>Galpidshypnyk_com, TEST 10.06.21</t>
+  </si>
+  <si>
+    <t>edge-199</t>
+  </si>
+  <si>
+    <t>3bd0057e-cc2f-4ce0-9ca8-42bc3a2e2845</t>
+  </si>
+  <si>
+    <t>vse-Dobronet EDGE (082ec285-168e-4419-a4fc-90641d2ce87f)</t>
+  </si>
+  <si>
+    <t>vse-60689a14-a346-44d4-a841-907923584d2a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ООО Добронет	 TEST 14.06.21	 Тростьяк Андрей Викторович sklif@dobronet.com.ua		 +380667860156</t>
+  </si>
+  <si>
+    <t>edge-200</t>
+  </si>
+  <si>
+    <t>889a4f76-6066-40a7-b771-a2f3cc017051</t>
+  </si>
+  <si>
+    <t>vse-Yukoil EDGE (81d3cda5-c566-48cc-b7a8-73212092e6a6)</t>
+  </si>
+  <si>
+    <t>vse-79cd1d34-0354-4159-b8ea-4a5f3b1821db</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ООО "СП Юкойл" TEST 18.06.2021 Матвеев Илья Евгеньевич  admin@yukoil.com    +380504888866</t>
+  </si>
+  <si>
+    <t>edge-201</t>
+  </si>
+  <si>
+    <t>01d3d0ec-d5ae-40d4-9d2b-0d623bf35036</t>
+  </si>
+  <si>
+    <t>vse-TSPS EDGE (ae2a4dba-2720-4a8e-a5b1-86f4848eb828)</t>
+  </si>
+  <si>
+    <t>vse-e3dc8b05-2044-4ca3-af31-d8eaad74d4f5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТОВ "ТСПС"	TEST 23.06.21 Сергій Басов  sergey@basov.in.ua	0504111191</t>
+  </si>
+  <si>
+    <t>edge-202</t>
+  </si>
+  <si>
+    <t>8b4803da-1d36-4bd6-972b-31da9ef17907</t>
+  </si>
+  <si>
+    <t>vse-CEK EDGE (42d2754f-8851-48dd-9a03-f6b8d7648859)</t>
+  </si>
+  <si>
+    <t>vse-da48a17a-bc66-4300-bef8-ddef53230481</t>
+  </si>
+  <si>
+    <t>ЦЕК. TEST start from 05.07.2021 Prusenko R., +380504577862, rprusenko@cek.dp.ua</t>
+  </si>
+  <si>
+    <t>edge-203</t>
+  </si>
+  <si>
+    <t>5cfd2de3-e6bd-4e18-84a4-c8c2d5fa25d0</t>
+  </si>
+  <si>
+    <t>vse-Ukrspirt EDGE (aca69261-1781-4f2a-9e2c-a3c68583ab78)</t>
+  </si>
+  <si>
+    <t>vse-def7bd05-1cbd-4301-a245-7f39262d1ce5</t>
+  </si>
+  <si>
+    <t>Ukrspirt Test 07.07.2021</t>
+  </si>
+  <si>
+    <t>edge-204</t>
+  </si>
+  <si>
+    <t>acc10e67-a389-4e32-9bdd-17c010284b1a</t>
+  </si>
+  <si>
+    <t>vse-Tandem EDGE (72280e5c-b446-4bcd-87ee-8ea65a1ea0b9)</t>
+  </si>
+  <si>
+    <t>vse-15867750-5b1a-4dc5-abf4-a420e720e636</t>
+  </si>
+  <si>
+    <t>Тандем 2002, TEST start from 09.07.2021 Artem Fetsenets, +380953311745, artem.fetsenets@edinstvo.ua</t>
+  </si>
+  <si>
+    <t>edge-205</t>
+  </si>
+  <si>
+    <t>e9524833-a8eb-412d-b9ad-0f3d2d1f85e9</t>
+  </si>
+  <si>
+    <t>vse-Alfa_Corp EDGE (755e26f2-5fa1-48c2-8570-bb473e8e6219)</t>
+  </si>
+  <si>
+    <t>vse-0075cb95-c845-4dd4-843d-167f201cc151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТОВ "АЛЬФА-ОБЕРЕГ" alfa_korp  TEST 12.07.21 Мелешин Георгий alfa_teh@ukr.net 067-644-3573, 096 085 074 6</t>
+  </si>
+  <si>
+    <t>edge-206</t>
+  </si>
+  <si>
+    <t>8652c275-1d71-45f2-b5d8-0ed9115f4f79</t>
+  </si>
+  <si>
+    <t>vse-Lubnygaz EDGE (0ef741a4-1d85-4027-9e58-0480b0943bb2)</t>
+  </si>
+  <si>
+    <t>vse-5389b7b3-10d3-4022-9179-306ec4011e5a</t>
+  </si>
+  <si>
+    <t>АТ Лубнигаз, Test start from 13.07.2021, Kolvasenko Vitalii, +380667704101, admin3@lubnygaz.com.ua</t>
+  </si>
+  <si>
+    <t>edge-208</t>
+  </si>
+  <si>
+    <t>fa396dee-37b0-4879-9e35-467c884a5cf9</t>
+  </si>
+  <si>
+    <t>vse-UKROLIYA_LTD EDGE (24a02774-70dc-468c-b424-0fd425a8397d)</t>
+  </si>
+  <si>
+    <t>vse-5ae270ab-8226-439d-aeac-201d79803c45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">УКРОЛИЯ UKROLIYA LTD TEST 19/07/21 Подолян Е.А. it@ukroliya.com +380504053666 </t>
+  </si>
+  <si>
+    <t>edge-211</t>
+  </si>
+  <si>
+    <t>b7ed8c4f-c49b-4210-928d-b832a92ea354</t>
+  </si>
+  <si>
+    <t>vse-Okolica EDGE (a201c0ba-ecb2-415f-adad-b65e374dbfb6)</t>
+  </si>
+  <si>
+    <t>vse-cae59409-b0d1-42aa-ab59-8bf6b01d2157</t>
+  </si>
+  <si>
+    <t>Okolica TEST 28.07.21</t>
+  </si>
+  <si>
+    <t>edge-212</t>
+  </si>
+  <si>
+    <t>c853a126-f40d-458c-a8a7-fa247d6688b8</t>
+  </si>
+  <si>
+    <t>vse-Svyataya Yekaterina EDGE (80d322b6-ed90-45f9-86c7-ee984f85bb4f)</t>
+  </si>
+  <si>
+    <t>vse-405b1a72-dc26-4069-bec8-92a7881efa59</t>
+  </si>
+  <si>
+    <t>Svyataya_Yekaterina, TEST 28.07.21</t>
+  </si>
+  <si>
+    <t>edge-213</t>
+  </si>
+  <si>
+    <t>6149175d-0114-4d44-a0be-ce1d3435decc</t>
+  </si>
+  <si>
+    <t>vse-NOBILITET EDGE (d892b358-0c7a-4375-9151-27dabb435496)</t>
+  </si>
+  <si>
+    <t>vse-08ed0ebe-5c33-4b80-b014-e41c189e6217</t>
+  </si>
+  <si>
+    <t>NOBILITET, PROD 02.08.21</t>
+  </si>
+  <si>
+    <t>edge-214</t>
+  </si>
+  <si>
+    <t>f844f59a-33d4-41c3-b29d-b606abca312b</t>
+  </si>
+  <si>
+    <t>vse-Cloud EDGE (81b3aba9-d2a8-4d9f-8eae-bb2b10467bb8)</t>
+  </si>
+  <si>
+    <t>vse-b466b36b-f64d-4555-be9d-d8132739d3ed</t>
+  </si>
+  <si>
+    <t>Cloud, TEST 10.08.21</t>
+  </si>
+  <si>
+    <t>edge-215</t>
+  </si>
+  <si>
+    <t>c8db3267-58c1-42b9-9120-7b7274aa3001</t>
+  </si>
+  <si>
+    <t>vse-AVK EDGE (2af3ea32-612e-4267-87af-55ec6fdb1d74)</t>
+  </si>
+  <si>
+    <t>vse-292dce39-0709-46f8-ae0a-1573754dc168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ЧАО АВК  TEST 13.08.21 Контактные данные ответственного лица заказчика: Шестаков Андрей Евгеньевич add-def@ukr.net 050-4811940</t>
+  </si>
+  <si>
+    <t>edge-216</t>
+  </si>
+  <si>
+    <t>f4ab1899-829f-4507-82a5-940c1078e024</t>
+  </si>
+  <si>
+    <t>vse-Betonmash EDGE (49da4e84-ccd1-4e8a-8321-5b4552131164)</t>
+  </si>
+  <si>
+    <t>vse-38b424ae-3add-4a34-9ea3-b41efab855cc</t>
+  </si>
+  <si>
+    <t>ЧАО "Бетонмаш" TEST 17.08.2021 Булгаков Ярослав Юрьевич, ivc@betonmash.com +380507111065</t>
+  </si>
+  <si>
+    <t>edge-217</t>
+  </si>
+  <si>
+    <t>e0300870-595f-498a-8769-1c42b38e8a8e</t>
+  </si>
+  <si>
+    <t>vse-Agrosat EDGE (8fca58e1-7df4-443f-b269-03536b5df6d2)</t>
+  </si>
+  <si>
+    <t>vse-70f52453-6f94-4a63-8dd1-19935868b8e1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТОВ АГРО-САТЕЛИТ TEST 17.08.21 agrosat   Вадим Голобородько info@smartland.in.ua 0667327379</t>
+  </si>
+  <si>
+    <t>edge-218</t>
+  </si>
+  <si>
+    <t>1b038523-38a1-4b98-83c9-8132e79888a1</t>
+  </si>
+  <si>
+    <t>vse-Mkl10 EDGE (9b0b9283-f64c-4c5f-9d5d-1924b864f431)</t>
+  </si>
+  <si>
+    <t>vse-df4e2760-3b3b-4582-841d-031292eb913e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">КНП "МКЛ № 10" ОМР  TEST 20.08.21 Максим Цыбульский; it@svekaterina.ua; 0503914540</t>
   </si>
   <si>
     <t>virtualServerId</t>
@@ -873,9 +1107,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -886,14 +1120,14 @@
     <col min="3" max="3" width="9.57164478302002" customWidth="1"/>
     <col min="4" max="4" width="15.933064460754395" customWidth="1"/>
     <col min="5" max="5" width="16.52644157409668" customWidth="1"/>
-    <col min="6" max="6" width="38.7535514831543" customWidth="1"/>
-    <col min="7" max="7" width="64.42533111572266" customWidth="1"/>
-    <col min="8" max="8" width="42.4273796081543" customWidth="1"/>
+    <col min="6" max="6" width="38.811866760253906" customWidth="1"/>
+    <col min="7" max="7" width="69.80563354492188" customWidth="1"/>
+    <col min="8" max="8" width="42.50615692138672" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
     <col min="10" max="10" width="15.931017875671387" customWidth="1"/>
     <col min="11" max="11" width="11.232078552246094" customWidth="1"/>
     <col min="12" max="12" width="16.114147186279297" customWidth="1"/>
-    <col min="13" max="13" width="116.3523941040039" customWidth="1"/>
+    <col min="13" max="13" width="136.0306854248047" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -983,7 +1217,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="0">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>14</v>
@@ -1106,7 +1340,7 @@
         <v>35</v>
       </c>
       <c r="B6" s="0">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>14</v>
@@ -1229,7 +1463,7 @@
         <v>47</v>
       </c>
       <c r="B9" s="0">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>14</v>
@@ -1393,7 +1627,7 @@
         <v>63</v>
       </c>
       <c r="B13" s="0">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>14</v>
@@ -1475,7 +1709,7 @@
         <v>71</v>
       </c>
       <c r="B15" s="0">
-        <v>1</v>
+        <v>138</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>14</v>
@@ -1516,7 +1750,7 @@
         <v>76</v>
       </c>
       <c r="B16" s="0">
-        <v>1</v>
+        <v>160</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>14</v>
@@ -1557,7 +1791,7 @@
         <v>81</v>
       </c>
       <c r="B17" s="0">
-        <v>137</v>
+        <v>28</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>14</v>
@@ -1598,7 +1832,7 @@
         <v>86</v>
       </c>
       <c r="B18" s="0">
-        <v>153</v>
+        <v>2</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>14</v>
@@ -1639,7 +1873,7 @@
         <v>91</v>
       </c>
       <c r="B19" s="0">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>14</v>
@@ -1680,7 +1914,7 @@
         <v>96</v>
       </c>
       <c r="B20" s="0">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>14</v>
@@ -1713,130 +1947,130 @@
         <v>21</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="0">
+        <v>18</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="B21" s="0">
-        <v>2</v>
-      </c>
-      <c r="C21" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="0" t="s">
+      <c r="G21" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="G21" s="0" t="s">
+      <c r="H21" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="I21" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="I21" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J21" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M21" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="0">
+        <v>3</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B22" s="0">
-        <v>29</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="0" t="s">
+      <c r="G22" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="H22" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="H22" s="0" t="s">
+      <c r="I22" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L22" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M22" s="0" t="s">
         <v>109</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J22" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M22" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="0">
+        <v>38</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="B23" s="0">
-        <v>45</v>
-      </c>
-      <c r="C23" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="0" t="s">
+      <c r="G23" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="H23" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="I23" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" s="0" t="s">
         <v>114</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J23" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L23" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M23" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="24">
@@ -1844,7 +2078,7 @@
         <v>115</v>
       </c>
       <c r="B24" s="0">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>14</v>
@@ -1885,7 +2119,7 @@
         <v>120</v>
       </c>
       <c r="B25" s="0">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>14</v>
@@ -1926,7 +2160,7 @@
         <v>125</v>
       </c>
       <c r="B26" s="0">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>14</v>
@@ -1967,7 +2201,7 @@
         <v>130</v>
       </c>
       <c r="B27" s="0">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>14</v>
@@ -2008,7 +2242,7 @@
         <v>135</v>
       </c>
       <c r="B28" s="0">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>14</v>
@@ -2049,7 +2283,7 @@
         <v>140</v>
       </c>
       <c r="B29" s="0">
-        <v>1</v>
+        <v>183</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>14</v>
@@ -2090,7 +2324,7 @@
         <v>145</v>
       </c>
       <c r="B30" s="0">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>14</v>
@@ -2102,14 +2336,14 @@
         <v>16</v>
       </c>
       <c r="F30" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="G30" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="G30" s="0" t="s">
+      <c r="H30" s="0" t="s">
         <v>147</v>
       </c>
-      <c r="H30" s="0" t="s">
-        <v>148</v>
-      </c>
       <c r="I30" s="0" t="s">
         <v>8</v>
       </c>
@@ -2123,499 +2357,499 @@
         <v>21</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>149</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B31" s="0">
+        <v>96</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="G31" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="B31" s="0">
-        <v>15</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="0" t="s">
+      <c r="H31" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="G31" s="0" t="s">
+      <c r="I31" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K31" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L31" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M31" s="0" t="s">
         <v>152</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J31" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K31" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L31" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M31" s="0" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B32" s="0">
+        <v>82</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="G32" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B32" s="0">
-        <v>1</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="0" t="s">
+      <c r="H32" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="G32" s="0" t="s">
+      <c r="I32" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K32" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L32" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M32" s="0" t="s">
         <v>157</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>158</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J32" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K32" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L32" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M32" s="0" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B33" s="0">
+        <v>13</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="G33" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="B33" s="0">
-        <v>33</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="0" t="s">
+      <c r="H33" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="G33" s="0" t="s">
+      <c r="I33" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L33" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" s="0" t="s">
         <v>162</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J33" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K33" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L33" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M33" s="0" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" s="0">
+        <v>87</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="G34" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="B34" s="0">
-        <v>226</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="0" t="s">
+      <c r="H34" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="G34" s="0" t="s">
+      <c r="I34" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L34" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M34" s="0" t="s">
         <v>167</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>168</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J34" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K34" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L34" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M34" s="0" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B35" s="0">
+        <v>81</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="G35" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="B35" s="0">
-        <v>3</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="0" t="s">
+      <c r="H35" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="G35" s="0" t="s">
+      <c r="I35" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K35" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L35" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M35" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>173</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J35" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K35" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L35" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M35" s="0" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="0">
+        <v>54</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>174</v>
+      </c>
+      <c r="G36" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="B36" s="0">
-        <v>7</v>
-      </c>
-      <c r="C36" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="0" t="s">
+      <c r="H36" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="G36" s="0" t="s">
+      <c r="I36" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K36" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M36" s="0" t="s">
         <v>177</v>
-      </c>
-      <c r="H36" s="0" t="s">
-        <v>178</v>
-      </c>
-      <c r="I36" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J36" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K36" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L36" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M36" s="0" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B37" s="0">
+        <v>25</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="G37" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="B37" s="0">
-        <v>24</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F37" s="0" t="s">
+      <c r="H37" s="0" t="s">
         <v>181</v>
       </c>
-      <c r="G37" s="0" t="s">
+      <c r="I37" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M37" s="0" t="s">
         <v>182</v>
-      </c>
-      <c r="H37" s="0" t="s">
-        <v>183</v>
-      </c>
-      <c r="I37" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J37" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K37" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L37" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M37" s="0" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" s="0">
+        <v>31</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E38" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="G38" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B38" s="0">
-        <v>1</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E38" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F38" s="0" t="s">
+      <c r="H38" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="G38" s="0" t="s">
+      <c r="I38" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K38" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L38" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M38" s="0" t="s">
         <v>187</v>
-      </c>
-      <c r="H38" s="0" t="s">
-        <v>188</v>
-      </c>
-      <c r="I38" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J38" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K38" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L38" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M38" s="0" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="B39" s="0">
+        <v>78</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="G39" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="B39" s="0">
-        <v>3</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E39" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="0" t="s">
+      <c r="H39" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="G39" s="0" t="s">
+      <c r="I39" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K39" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L39" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M39" s="0" t="s">
         <v>192</v>
-      </c>
-      <c r="H39" s="0" t="s">
-        <v>193</v>
-      </c>
-      <c r="I39" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J39" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K39" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L39" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M39" s="0" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="B40" s="0">
+        <v>1</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="G40" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="B40" s="0">
-        <v>16</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E40" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="0" t="s">
+      <c r="H40" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="G40" s="0" t="s">
+      <c r="I40" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K40" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L40" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M40" s="0" t="s">
         <v>197</v>
-      </c>
-      <c r="H40" s="0" t="s">
-        <v>198</v>
-      </c>
-      <c r="I40" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J40" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K40" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L40" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M40" s="0" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="s">
+        <v>198</v>
+      </c>
+      <c r="B41" s="0">
+        <v>1</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>199</v>
+      </c>
+      <c r="G41" s="0" t="s">
         <v>200</v>
       </c>
-      <c r="B41" s="0">
-        <v>99</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="0" t="s">
+      <c r="H41" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="G41" s="0" t="s">
+      <c r="I41" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L41" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M41" s="0" t="s">
         <v>202</v>
-      </c>
-      <c r="H41" s="0" t="s">
-        <v>203</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J41" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K41" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L41" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M41" s="0" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B42" s="0">
+        <v>1</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E42" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="G42" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="B42" s="0">
-        <v>4</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E42" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F42" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="G42" s="0" t="s">
+      <c r="H42" s="0" t="s">
         <v>206</v>
       </c>
-      <c r="H42" s="0" t="s">
+      <c r="I42" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K42" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L42" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M42" s="0" t="s">
         <v>207</v>
-      </c>
-      <c r="I42" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J42" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K42" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L42" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M42" s="0" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="43">
@@ -2623,7 +2857,7 @@
         <v>208</v>
       </c>
       <c r="B43" s="0">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>14</v>
@@ -2664,7 +2898,7 @@
         <v>213</v>
       </c>
       <c r="B44" s="0">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>14</v>
@@ -2705,7 +2939,7 @@
         <v>218</v>
       </c>
       <c r="B45" s="0">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>14</v>
@@ -2717,13 +2951,13 @@
         <v>16</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>209</v>
+        <v>219</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I45" s="0" t="s">
         <v>8</v>
@@ -2738,15 +2972,15 @@
         <v>21</v>
       </c>
       <c r="M45" s="0" t="s">
-        <v>27</v>
+        <v>222</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="B46" s="0">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>14</v>
@@ -2758,13 +2992,13 @@
         <v>16</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="I46" s="0" t="s">
         <v>8</v>
@@ -2779,15 +3013,15 @@
         <v>21</v>
       </c>
       <c r="M46" s="0" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B47" s="0">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>14</v>
@@ -2799,13 +3033,13 @@
         <v>16</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="I47" s="0" t="s">
         <v>8</v>
@@ -2820,15 +3054,15 @@
         <v>21</v>
       </c>
       <c r="M47" s="0" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B48" s="0">
-        <v>55</v>
+        <v>1</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>14</v>
@@ -2840,13 +3074,13 @@
         <v>16</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="I48" s="0" t="s">
         <v>8</v>
@@ -2861,15 +3095,15 @@
         <v>21</v>
       </c>
       <c r="M48" s="0" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B49" s="0">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>14</v>
@@ -2881,13 +3115,13 @@
         <v>16</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="I49" s="0" t="s">
         <v>8</v>
@@ -2902,12 +3136,12 @@
         <v>21</v>
       </c>
       <c r="M49" s="0" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B50" s="0">
         <v>1</v>
@@ -2922,13 +3156,13 @@
         <v>16</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="I50" s="0" t="s">
         <v>8</v>
@@ -2943,15 +3177,15 @@
         <v>21</v>
       </c>
       <c r="M50" s="0" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B51" s="0">
-        <v>1</v>
+        <v>61</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>14</v>
@@ -2963,13 +3197,13 @@
         <v>16</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="I51" s="0" t="s">
         <v>8</v>
@@ -2984,48 +3218,663 @@
         <v>21</v>
       </c>
       <c r="M51" s="0" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B52" s="0">
+        <v>31</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="G52" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="H52" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="I52" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K52" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L52" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M52" s="0" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="B53" s="0">
         <v>1</v>
       </c>
-      <c r="C52" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F52" s="0" t="s">
-        <v>252</v>
-      </c>
-      <c r="G52" s="0" t="s">
-        <v>253</v>
-      </c>
-      <c r="H52" s="0" t="s">
-        <v>254</v>
-      </c>
-      <c r="I52" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="J52" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="K52" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="L52" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="M52" s="0" t="s">
-        <v>27</v>
+      <c r="C53" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="G53" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="H53" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="I53" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" s="0" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="B54" s="0">
+        <v>17</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="G54" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="H54" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="I54" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L54" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M54" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="B55" s="0">
+        <v>7</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="G55" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="H55" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="I55" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K55" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L55" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M55" s="0" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B56" s="0">
+        <v>2</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="G56" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="H56" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="I56" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K56" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L56" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M56" s="0" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="B57" s="0">
+        <v>31</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D57" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="G57" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="H57" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="I57" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K57" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L57" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M57" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="B58" s="0">
+        <v>1</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="G58" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="H58" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="I58" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K58" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L58" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M58" s="0" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="B59" s="0">
+        <v>17</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="G59" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="H59" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="I59" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K59" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L59" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M59" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="B60" s="0">
+        <v>4</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E60" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F60" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="G60" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="H60" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="I60" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J60" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K60" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L60" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M60" s="0" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="B61" s="0">
+        <v>32</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E61" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="G61" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="H61" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="I61" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K61" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L61" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M61" s="0" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="B62" s="0">
+        <v>16</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E62" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F62" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="G62" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="H62" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="I62" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J62" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K62" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L62" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M62" s="0" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B63" s="0">
+        <v>53</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="G63" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="H63" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="I63" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K63" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L63" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M63" s="0" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="B64" s="0">
+        <v>11</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D64" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F64" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="G64" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="H64" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="I64" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L64" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M64" s="0" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="B65" s="0">
+        <v>1</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="G65" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="H65" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="I65" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K65" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L65" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M65" s="0" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="B66" s="0">
+        <v>1</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="0" t="s">
+        <v>324</v>
+      </c>
+      <c r="G66" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="H66" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="I66" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K66" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L66" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M66" s="0" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="B67" s="0">
+        <v>1</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F67" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="G67" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="H67" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="I67" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J67" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="K67" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L67" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M67" s="0" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -3033,9 +3882,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3058,48 +3907,48 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>255</v>
+        <v>333</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>256</v>
+        <v>334</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>257</v>
+        <v>335</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>258</v>
+        <v>336</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>259</v>
+        <v>337</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>260</v>
+        <v>338</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>261</v>
+        <v>339</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>262</v>
+        <v>340</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>263</v>
+        <v>341</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>264</v>
+        <v>342</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>265</v>
+        <v>343</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>266</v>
+        <v>344</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>267</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>21</v>
@@ -3116,7 +3965,7 @@
     </row>
     <row r="3">
       <c r="B3" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>21</v>
@@ -3133,7 +3982,7 @@
     </row>
     <row r="4">
       <c r="B4" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>21</v>
@@ -3150,7 +3999,7 @@
     </row>
     <row r="5">
       <c r="B5" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>21</v>
@@ -3167,7 +4016,7 @@
     </row>
     <row r="6">
       <c r="B6" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>21</v>
@@ -3184,7 +4033,7 @@
     </row>
     <row r="7">
       <c r="B7" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>21</v>
@@ -3201,7 +4050,7 @@
     </row>
     <row r="8">
       <c r="B8" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>21</v>
@@ -3218,7 +4067,7 @@
     </row>
     <row r="9">
       <c r="B9" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>21</v>
@@ -3235,7 +4084,7 @@
     </row>
     <row r="10">
       <c r="B10" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>21</v>
@@ -3252,7 +4101,7 @@
     </row>
     <row r="11">
       <c r="B11" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>21</v>
@@ -3269,7 +4118,7 @@
     </row>
     <row r="12">
       <c r="B12" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>21</v>
@@ -3286,7 +4135,7 @@
     </row>
     <row r="13">
       <c r="B13" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>21</v>
@@ -3303,7 +4152,7 @@
     </row>
     <row r="14">
       <c r="B14" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>21</v>
@@ -3320,7 +4169,7 @@
     </row>
     <row r="15">
       <c r="B15" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>21</v>
@@ -3329,7 +4178,7 @@
         <v>21</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>21</v>
+        <v>347</v>
       </c>
       <c r="M15" s="0" t="s">
         <v>27</v>
@@ -3337,7 +4186,7 @@
     </row>
     <row r="16">
       <c r="B16" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>21</v>
@@ -3354,7 +4203,7 @@
     </row>
     <row r="17">
       <c r="B17" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>21</v>
@@ -3363,7 +4212,7 @@
         <v>21</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>269</v>
+        <v>21</v>
       </c>
       <c r="M17" s="0" t="s">
         <v>27</v>
@@ -3371,7 +4220,7 @@
     </row>
     <row r="18">
       <c r="B18" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>21</v>
@@ -3388,7 +4237,7 @@
     </row>
     <row r="19">
       <c r="B19" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>21</v>
@@ -3405,7 +4254,7 @@
     </row>
     <row r="20">
       <c r="B20" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>21</v>
@@ -3422,7 +4271,7 @@
     </row>
     <row r="21">
       <c r="B21" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>21</v>
@@ -3439,7 +4288,7 @@
     </row>
     <row r="22">
       <c r="B22" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>21</v>
@@ -3456,7 +4305,7 @@
     </row>
     <row r="23">
       <c r="B23" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>21</v>
@@ -3473,7 +4322,7 @@
     </row>
     <row r="24">
       <c r="B24" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>21</v>
@@ -3490,7 +4339,7 @@
     </row>
     <row r="25">
       <c r="B25" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>21</v>
@@ -3507,7 +4356,7 @@
     </row>
     <row r="26">
       <c r="B26" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>21</v>
@@ -3524,7 +4373,7 @@
     </row>
     <row r="27">
       <c r="B27" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>21</v>
@@ -3541,7 +4390,7 @@
     </row>
     <row r="28">
       <c r="B28" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>21</v>
@@ -3558,7 +4407,7 @@
     </row>
     <row r="29">
       <c r="B29" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>21</v>
@@ -3575,7 +4424,7 @@
     </row>
     <row r="30">
       <c r="B30" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>21</v>
@@ -3592,7 +4441,7 @@
     </row>
     <row r="31">
       <c r="B31" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>21</v>
@@ -3609,7 +4458,7 @@
     </row>
     <row r="32">
       <c r="B32" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>21</v>
@@ -3626,7 +4475,7 @@
     </row>
     <row r="33">
       <c r="B33" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C33" s="0" t="s">
         <v>21</v>
@@ -3643,7 +4492,7 @@
     </row>
     <row r="34">
       <c r="B34" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C34" s="0" t="s">
         <v>21</v>
@@ -3660,7 +4509,7 @@
     </row>
     <row r="35">
       <c r="B35" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C35" s="0" t="s">
         <v>21</v>
@@ -3677,7 +4526,7 @@
     </row>
     <row r="36">
       <c r="B36" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C36" s="0" t="s">
         <v>21</v>
@@ -3694,7 +4543,7 @@
     </row>
     <row r="37">
       <c r="B37" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C37" s="0" t="s">
         <v>21</v>
@@ -3711,7 +4560,7 @@
     </row>
     <row r="38">
       <c r="B38" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C38" s="0" t="s">
         <v>21</v>
@@ -3728,7 +4577,7 @@
     </row>
     <row r="39">
       <c r="B39" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C39" s="0" t="s">
         <v>21</v>
@@ -3745,7 +4594,7 @@
     </row>
     <row r="40">
       <c r="B40" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C40" s="0" t="s">
         <v>21</v>
@@ -3762,7 +4611,7 @@
     </row>
     <row r="41">
       <c r="B41" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C41" s="0" t="s">
         <v>21</v>
@@ -3779,7 +4628,7 @@
     </row>
     <row r="42">
       <c r="B42" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C42" s="0" t="s">
         <v>21</v>
@@ -3796,7 +4645,7 @@
     </row>
     <row r="43">
       <c r="B43" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C43" s="0" t="s">
         <v>21</v>
@@ -3813,7 +4662,7 @@
     </row>
     <row r="44">
       <c r="B44" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C44" s="0" t="s">
         <v>21</v>
@@ -3830,7 +4679,7 @@
     </row>
     <row r="45">
       <c r="B45" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C45" s="0" t="s">
         <v>21</v>
@@ -3847,7 +4696,7 @@
     </row>
     <row r="46">
       <c r="B46" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C46" s="0" t="s">
         <v>21</v>
@@ -3864,7 +4713,7 @@
     </row>
     <row r="47">
       <c r="B47" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C47" s="0" t="s">
         <v>21</v>
@@ -3881,7 +4730,7 @@
     </row>
     <row r="48">
       <c r="B48" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C48" s="0" t="s">
         <v>21</v>
@@ -3898,7 +4747,7 @@
     </row>
     <row r="49">
       <c r="B49" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C49" s="0" t="s">
         <v>21</v>
@@ -3915,7 +4764,7 @@
     </row>
     <row r="50">
       <c r="B50" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C50" s="0" t="s">
         <v>21</v>
@@ -3932,7 +4781,7 @@
     </row>
     <row r="51">
       <c r="B51" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C51" s="0" t="s">
         <v>21</v>
@@ -3949,7 +4798,7 @@
     </row>
     <row r="52">
       <c r="B52" s="0" t="s">
-        <v>268</v>
+        <v>346</v>
       </c>
       <c r="C52" s="0" t="s">
         <v>21</v>
@@ -3961,6 +4810,261 @@
         <v>21</v>
       </c>
       <c r="M52" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M53" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K54" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L54" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M54" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K55" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L55" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M55" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K56" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L56" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M56" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C57" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K57" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L57" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M57" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C58" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K58" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L58" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M58" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K59" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L59" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M59" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K60" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L60" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M60" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K61" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L61" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M61" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K62" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L62" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M62" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K63" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L63" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M63" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C64" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K64" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L64" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M64" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K65" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L65" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M65" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K66" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L66" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M66" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K67" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="L67" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="M67" s="0" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>